<commit_message>
deafault rate max rate for services
</commit_message>
<xml_diff>
--- a/gkwebapp/static/spreadsheets/Product_Import_Sample_Spreadsheet.xlsx
+++ b/gkwebapp/static/spreadsheets/Product_Import_Sample_Spreadsheet.xlsx
@@ -31,10 +31,10 @@
     <t xml:space="preserve">Unit of Measurement</t>
   </si>
   <si>
-    <t xml:space="preserve">Mrp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sale Price</t>
+    <t xml:space="preserve">Mrp / Maximum Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sale Price / Default Rate</t>
   </si>
   <si>
     <t xml:space="preserve">Tax</t>
@@ -192,12 +192,17 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -323,6 +328,12 @@
       </c>
       <c r="B6" s="0" t="n">
         <v>23</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>450</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Modified product sample spreadsheet
</commit_message>
<xml_diff>
--- a/gkwebapp/static/spreadsheets/Product_Import_Sample_Spreadsheet.xlsx
+++ b/gkwebapp/static/spreadsheets/Product_Import_Sample_Spreadsheet.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t xml:space="preserve">Product Name</t>
   </si>
   <si>
-    <t xml:space="preserve">HSN Code</t>
+    <t xml:space="preserve">HSN/ SAC Code</t>
   </si>
   <si>
     <t xml:space="preserve">Unit of Measurement</t>
@@ -37,6 +37,12 @@
     <t xml:space="preserve">Sale Price / Default Rate</t>
   </si>
   <si>
+    <t xml:space="preserve">Discout Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discount Percent(%)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tax</t>
   </si>
   <si>
@@ -52,7 +58,7 @@
     <t xml:space="preserve">Opening Stock</t>
   </si>
   <si>
-    <t xml:space="preserve">Product 1</t>
+    <t xml:space="preserve">Product 12001</t>
   </si>
   <si>
     <t xml:space="preserve">BAG</t>
@@ -61,34 +67,31 @@
     <t xml:space="preserve">GST</t>
   </si>
   <si>
+    <t xml:space="preserve">VAT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maharashtra</t>
   </si>
   <si>
-    <t xml:space="preserve">VAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product 2</t>
+    <t xml:space="preserve">Product 23001</t>
   </si>
   <si>
     <t xml:space="preserve">BUNDLES</t>
   </si>
   <si>
-    <t xml:space="preserve">Punjab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Godown 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Godown 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service 2</t>
+    <t xml:space="preserve">Kurla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service 15001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service 26001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVAT</t>
   </si>
 </sst>
 </file>
@@ -174,12 +177,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -189,20 +192,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -236,59 +241,68 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>200</v>
+        <v>750</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="L2" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>50</v>
@@ -296,35 +310,32 @@
       <c r="E4" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="0" t="n">
+      <c r="K4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="0" t="n">
+      <c r="K5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>23</v>
@@ -333,30 +344,33 @@
         <v>500</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>450</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="0" t="n">
+        <v>475</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="K7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -365,38 +379,20 @@
       <c r="B8" s="0" t="n">
         <v>2370</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="H8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>12</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="H9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>6.6</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>